<commit_message>
Обновленный сервер Signed-off-by: Yulia Mahonina <yulya.machonina@mail.ru>
</commit_message>
<xml_diff>
--- a/coffe-app/ServerCoffeeApp/Users.xlsx
+++ b/coffe-app/ServerCoffeeApp/Users.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\KP_KPO\coffe-landishi\coffe-app\ServerCoffeeApp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ABB066D-2A10-4BD1-BADB-2C75416EE07C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{486C9D0C-B795-40C7-8B34-8193E915C674}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,21 +25,33 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>number</t>
+  </si>
   <si>
     <t>e-mail</t>
   </si>
   <si>
-    <t>number</t>
-  </si>
-  <si>
-    <t>username</t>
-  </si>
-  <si>
     <t>date</t>
   </si>
   <si>
     <t>password</t>
+  </si>
+  <si>
+    <t>youlchikk</t>
+  </si>
+  <si>
+    <t>3863055</t>
+  </si>
+  <si>
+    <t>yulia@mail.ru</t>
+  </si>
+  <si>
+    <t>06-05-2004</t>
   </si>
 </sst>
 </file>
@@ -357,32 +369,52 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15.6640625" customWidth="1"/>
-    <col min="2" max="2" width="15.33203125" customWidth="1"/>
+    <col min="2" max="2" width="16.77734375" customWidth="1"/>
+    <col min="3" max="3" width="18.5546875" customWidth="1"/>
+    <col min="4" max="4" width="17.44140625" customWidth="1"/>
+    <col min="5" max="5" width="16.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>